<commit_message>
Update results & plot timescale
</commit_message>
<xml_diff>
--- a/Ages.xlsx
+++ b/Ages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjjg18\GitHub\phylo-vetu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D5694E-7951-4F07-9CC7-2B8643794C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF7610BE-6CE1-42E9-9730-E5A98303E70E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16110" yWindow="-15" windowWidth="16080" windowHeight="19245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="151">
   <si>
     <t>Herpetogaster collinsi</t>
   </si>
@@ -423,9 +423,6 @@
     <t>loTime</t>
   </si>
   <si>
-    <t>Latham Shale</t>
-  </si>
-  <si>
     <t>Drumian</t>
   </si>
   <si>
@@ -487,6 +484,12 @@
   </si>
   <si>
     <t>Galgenberg Fm, early Agdzian</t>
+  </si>
+  <si>
+    <t>Latham Shale, Bonnia-Olenella zone</t>
+  </si>
+  <si>
+    <t>Durham1978jp; Smith2013nc</t>
   </si>
 </sst>
 </file>
@@ -807,7 +810,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +858,7 @@
         <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F2">
         <v>508</v>
@@ -917,7 +920,7 @@
         <v>30</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5">
         <v>518</v>
@@ -931,7 +934,7 @@
         <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F6">
         <v>518</v>
@@ -948,7 +951,7 @@
         <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F7">
         <v>508</v>
@@ -965,7 +968,7 @@
         <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F8">
         <v>508</v>
@@ -982,7 +985,7 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9">
         <v>508</v>
@@ -1080,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F14">
         <v>508</v>
@@ -1094,13 +1097,13 @@
         <v>91</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F15">
         <v>518</v>
       </c>
       <c r="I15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1111,7 +1114,7 @@
         <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F16">
         <v>508</v>
@@ -1125,13 +1128,13 @@
         <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F17">
         <v>508</v>
       </c>
       <c r="I17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1142,13 +1145,13 @@
         <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18">
         <v>508</v>
       </c>
       <c r="I18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1159,13 +1162,13 @@
         <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F19">
         <v>508</v>
       </c>
       <c r="I19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1269,7 +1272,7 @@
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25">
         <v>504</v>
@@ -1289,7 +1292,7 @@
         <v>117</v>
       </c>
       <c r="E26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F26">
         <v>500</v>
@@ -1309,14 +1312,14 @@
         <v>118</v>
       </c>
       <c r="E27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F27">
         <f>VLOOKUP(E27, lookup!$A$1:$B$14, 2)</f>
         <v>474</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1333,13 +1336,13 @@
         <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28">
         <v>507</v>
       </c>
       <c r="I28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1390,13 +1393,13 @@
         <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F31">
         <v>509</v>
       </c>
       <c r="I31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,13 +1430,13 @@
         <v>40</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F33">
         <v>506</v>
       </c>
       <c r="G33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H33">
         <v>500</v>
@@ -1471,13 +1474,13 @@
         <v>40</v>
       </c>
       <c r="E35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F35">
         <v>508</v>
       </c>
       <c r="I35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -1509,13 +1512,13 @@
         <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F37">
         <v>511</v>
       </c>
       <c r="G37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H37">
         <v>505</v>
@@ -1535,19 +1538,19 @@
         <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F38">
         <v>508.5</v>
       </c>
       <c r="G38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H38">
         <v>507</v>
       </c>
       <c r="I38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1584,19 +1587,19 @@
         <v>42</v>
       </c>
       <c r="E40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F40">
         <v>512</v>
       </c>
       <c r="G40" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H40">
         <v>505</v>
       </c>
       <c r="I40" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1630,20 +1633,19 @@
         <v>40</v>
       </c>
       <c r="E42" t="s">
+        <v>149</v>
+      </c>
+      <c r="F42">
+        <v>512</v>
+      </c>
+      <c r="G42" t="s">
         <v>128</v>
-      </c>
-      <c r="F42">
-        <f>VLOOKUP(E42, lookup!$A$1:$B$14, 2)</f>
-        <v>408</v>
-      </c>
-      <c r="G42" t="s">
-        <v>129</v>
       </c>
       <c r="H42">
         <v>502</v>
       </c>
       <c r="I42" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1812,7 +1814,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B15">
         <v>508</v>
@@ -1820,7 +1822,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B16">
         <v>518</v>

</xml_diff>